<commit_message>
Removed redundant test files and adjusted unit tests accordingly
</commit_message>
<xml_diff>
--- a/test-files/adjacency-matrix-modifications/asymmetric-gene-order-input.xlsx
+++ b/test-files/adjacency-matrix-modifications/asymmetric-gene-order-input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="10620" tabRatio="831" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="25440" windowHeight="13840" tabRatio="831" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -201,6 +201,17 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -222,21 +233,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2336,7 +2368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
@@ -4374,8 +4406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4403,7 +4435,7 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
@@ -4412,19 +4444,19 @@
         <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
-        <v>25</v>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
-        <v>29</v>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="P1" t="s">
         <v>31</v>
@@ -4432,8 +4464,8 @@
       <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
-        <v>35</v>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="S1" t="s">
         <v>37</v>
@@ -4442,7 +4474,7 @@
         <v>39</v>
       </c>
       <c r="U1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="V1" t="s">
         <v>43</v>
@@ -5877,6 +5909,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Finish rework to testing framework. Edit files that were causing unintentional errors.
</commit_message>
<xml_diff>
--- a/test-files/adjacency-matrix-modifications/asymmetric-gene-order-input.xlsx
+++ b/test-files/adjacency-matrix-modifications/asymmetric-gene-order-input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>